<commit_message>
Add new Excel writing functionality and update tests
This commit introduces new files for writing to Excel, including examples for creating multiplication tables and appending data to existing sheets. Also, some existing test files have been renamed and reformatted for better readability and organization.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/Carpim.xlsx
+++ b/src/test/java/ApachePOI/resource/Carpim.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TechnoStudy\IdeaProjects\Cucumber7\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,11 +24,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>1x1=1</t>
+  </si>
+  <si>
+    <t>1x2=2</t>
+  </si>
+  <si>
+    <t>1x3=3</t>
+  </si>
+  <si>
+    <t>1x4=4</t>
+  </si>
+  <si>
+    <t>1x5=5</t>
+  </si>
+  <si>
+    <t>1x6=6</t>
+  </si>
+  <si>
+    <t>1x7=7</t>
+  </si>
+  <si>
+    <t>1x8=8</t>
+  </si>
+  <si>
+    <t>1x9=9</t>
+  </si>
+  <si>
+    <t>1x10=10</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,12 +372,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>